<commit_message>
major changes in examples processing
</commit_message>
<xml_diff>
--- a/data/compleat_wiki_man.xlsx
+++ b/data/compleat_wiki_man.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe\Documents\GitHub\PhyrexianDictionary\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EBDD32-8CFB-4D67-BEE3-3620A60FE385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD41FBDA-6126-4864-856C-82D51992C9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2014" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="866">
   <si>
     <t>IPA</t>
   </si>
@@ -2477,12 +2477,6 @@
     <t>Indicative, Present</t>
   </si>
   <si>
-    <t>mood</t>
-  </si>
-  <si>
-    <t>particle</t>
-  </si>
-  <si>
     <t>'u</t>
   </si>
   <si>
@@ -2537,9 +2531,6 @@
     <t>Alternative (or)</t>
   </si>
   <si>
-    <t>mood, suffix</t>
-  </si>
-  <si>
     <t>xə</t>
   </si>
   <si>
@@ -2552,21 +2543,12 @@
     <t>Negative (un-, not)</t>
   </si>
   <si>
-    <t>mood, prefix</t>
-  </si>
-  <si>
     <t>əl</t>
   </si>
   <si>
     <t>negative (anti-affirmative/double negative)</t>
   </si>
   <si>
-    <t>'a</t>
-  </si>
-  <si>
-    <t>ʔa</t>
-  </si>
-  <si>
     <t>obligation/necessity (must)</t>
   </si>
   <si>
@@ -2636,196 +2618,19 @@
     <t>Paired with past</t>
   </si>
   <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>to (spatial)</t>
-  </si>
-  <si>
-    <t>prefix</t>
-  </si>
-  <si>
-    <t>əšq</t>
-  </si>
-  <si>
-    <t>əʃq</t>
-  </si>
-  <si>
-    <t>on (spatial)</t>
-  </si>
-  <si>
-    <t>dl</t>
-  </si>
-  <si>
-    <t>in (spatial)</t>
-  </si>
-  <si>
-    <t>φɒ'</t>
-  </si>
-  <si>
-    <t>φɒʔ</t>
-  </si>
-  <si>
-    <t>until (temporal)</t>
-  </si>
-  <si>
-    <t>for (temporal)</t>
-  </si>
-  <si>
-    <t>'ɒp</t>
-  </si>
-  <si>
-    <t>ʔɒp</t>
-  </si>
-  <si>
-    <t>any</t>
-  </si>
-  <si>
-    <t>ɢə</t>
-  </si>
-  <si>
-    <t>this/that</t>
-  </si>
-  <si>
-    <t>ɣẅ</t>
-  </si>
-  <si>
-    <t>ɣɯ</t>
-  </si>
-  <si>
-    <t>from</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>of</t>
-  </si>
-  <si>
-    <t>qər</t>
-  </si>
-  <si>
-    <t>with</t>
-  </si>
-  <si>
-    <t>gr</t>
-  </si>
-  <si>
-    <t>than</t>
-  </si>
-  <si>
-    <t>prefix, suffix</t>
-  </si>
-  <si>
-    <t>pl</t>
-  </si>
-  <si>
-    <t>completion</t>
-  </si>
-  <si>
-    <t>plθ</t>
-  </si>
-  <si>
-    <t>not-completion</t>
-  </si>
-  <si>
-    <t>pn</t>
-  </si>
-  <si>
-    <t>greater</t>
-  </si>
-  <si>
-    <t>ke</t>
-  </si>
-  <si>
-    <t>collective</t>
-  </si>
-  <si>
-    <t>ɣwi</t>
-  </si>
-  <si>
-    <t>ability</t>
-  </si>
-  <si>
-    <t>tč</t>
-  </si>
-  <si>
-    <t>ttʃ</t>
-  </si>
-  <si>
-    <t>indicate order</t>
-  </si>
-  <si>
-    <t>suffix</t>
-  </si>
-  <si>
-    <t>xe_'ə</t>
-  </si>
-  <si>
-    <t>xe_ʔə</t>
-  </si>
-  <si>
-    <t>indicate frequency</t>
-  </si>
-  <si>
     <t>poor</t>
   </si>
   <si>
-    <t>'return this to your hand'</t>
-  </si>
-  <si>
-    <t>'put a counter on this'</t>
-  </si>
-  <si>
-    <t>'target card in your graveyard'</t>
-  </si>
-  <si>
-    <t>'until your next turn'</t>
-  </si>
-  <si>
-    <t>'you can do this for this turn'</t>
-  </si>
-  <si>
-    <t>'produce mana of any type'</t>
-  </si>
-  <si>
-    <t>'sacrifice this creature'</t>
-  </si>
-  <si>
-    <t>'a card from your deck'</t>
-  </si>
-  <si>
-    <t>'ability of a permanent'</t>
-  </si>
-  <si>
-    <t>'destroy all permanents with counters'</t>
-  </si>
-  <si>
-    <t>'more/less than'</t>
-  </si>
-  <si>
-    <t>'Complete (prefix + make)'</t>
-  </si>
-  <si>
-    <t>'half, rounded down (prefix + not + two + amounts)'</t>
-  </si>
-  <si>
-    <t>'Vigilance (ability + prefix + see)'</t>
-  </si>
-  <si>
-    <t>'world (prefix + land)'</t>
-  </si>
-  <si>
-    <t>'Immortality (prefix + un + death)'</t>
-  </si>
-  <si>
-    <t>Number-related. 'Top (first) card of your library '</t>
-  </si>
-  <si>
-    <t>Number-related. 'once per turn'</t>
-  </si>
-  <si>
     <t>'Unless'</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>ha</t>
+  </si>
+  <si>
+    <t>marker</t>
   </si>
 </sst>
 </file>
@@ -3226,8 +3031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A263" workbookViewId="0">
-      <selection activeCell="G234" sqref="G234:G280"/>
+    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
+      <selection activeCell="J242" sqref="J242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6365,7 +6170,7 @@
         <v>1</v>
       </c>
       <c r="K110" t="s">
-        <v>581</v>
+        <v>863</v>
       </c>
       <c r="L110" t="s">
         <v>809</v>
@@ -6394,7 +6199,7 @@
         <v>1</v>
       </c>
       <c r="K111" t="s">
-        <v>581</v>
+        <v>863</v>
       </c>
       <c r="L111" t="s">
         <v>809</v>
@@ -6423,7 +6228,7 @@
         <v>1</v>
       </c>
       <c r="K112" t="s">
-        <v>581</v>
+        <v>863</v>
       </c>
       <c r="L112" t="s">
         <v>809</v>
@@ -10090,14 +9895,11 @@
       <c r="F242" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H242" t="s">
-        <v>814</v>
-      </c>
       <c r="I242" t="b">
         <v>1</v>
       </c>
       <c r="K242" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L242" t="s">
         <v>809</v>
@@ -10105,31 +9907,28 @@
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
+        <v>814</v>
+      </c>
+      <c r="B243" t="s">
+        <v>815</v>
+      </c>
+      <c r="C243" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D243" s="5" t="s">
         <v>816</v>
       </c>
-      <c r="B243" t="s">
-        <v>817</v>
-      </c>
-      <c r="C243" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D243" s="5" t="s">
-        <v>818</v>
-      </c>
       <c r="E243" s="5" t="b">
         <v>0</v>
       </c>
       <c r="F243" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H243" t="s">
-        <v>814</v>
-      </c>
       <c r="I243" t="b">
         <v>1</v>
       </c>
       <c r="K243" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L243" t="s">
         <v>809</v>
@@ -10137,16 +9936,16 @@
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="B244" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C244" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D244" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="E244" s="5" t="b">
         <v>0</v>
@@ -10154,14 +9953,11 @@
       <c r="F244" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H244" t="s">
-        <v>814</v>
-      </c>
       <c r="I244" t="b">
         <v>1</v>
       </c>
       <c r="K244" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L244" t="s">
         <v>809</v>
@@ -10169,31 +9965,28 @@
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
+        <v>819</v>
+      </c>
+      <c r="B245" t="s">
+        <v>820</v>
+      </c>
+      <c r="C245" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D245" s="5" t="s">
         <v>821</v>
       </c>
-      <c r="B245" t="s">
-        <v>822</v>
-      </c>
-      <c r="C245" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D245" s="5" t="s">
-        <v>823</v>
-      </c>
       <c r="E245" s="5" t="b">
         <v>0</v>
       </c>
       <c r="F245" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H245" t="s">
-        <v>814</v>
-      </c>
       <c r="I245" t="b">
         <v>1</v>
       </c>
       <c r="K245" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L245" t="s">
         <v>809</v>
@@ -10201,16 +9994,16 @@
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B246" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="C246" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D246" s="5" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="E246" s="5" t="b">
         <v>0</v>
@@ -10218,14 +10011,11 @@
       <c r="F246" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H246" t="s">
-        <v>814</v>
-      </c>
       <c r="I246" t="b">
         <v>1</v>
       </c>
       <c r="K246" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L246" t="s">
         <v>809</v>
@@ -10233,16 +10023,16 @@
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B247" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="C247" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D247" s="5" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="E247" s="5" t="b">
         <v>0</v>
@@ -10250,14 +10040,11 @@
       <c r="F247" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H247" t="s">
-        <v>814</v>
-      </c>
       <c r="I247" t="b">
         <v>1</v>
       </c>
       <c r="K247" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L247" t="s">
         <v>809</v>
@@ -10265,16 +10052,16 @@
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B248" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="C248" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D248" s="5" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="E248" s="5" t="b">
         <v>0</v>
@@ -10282,14 +10069,11 @@
       <c r="F248" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H248" t="s">
-        <v>814</v>
-      </c>
       <c r="I248" t="b">
         <v>1</v>
       </c>
       <c r="K248" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L248" t="s">
         <v>809</v>
@@ -10297,16 +10081,16 @@
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B249" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="C249" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D249" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="E249" s="5" t="b">
         <v>0</v>
@@ -10314,14 +10098,11 @@
       <c r="F249" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H249" t="s">
-        <v>814</v>
-      </c>
       <c r="I249" t="b">
         <v>1</v>
       </c>
       <c r="K249" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L249" t="s">
         <v>809</v>
@@ -10329,16 +10110,16 @@
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B250" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="C250" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D250" s="5" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="E250" s="5" t="b">
         <v>0</v>
@@ -10346,14 +10127,11 @@
       <c r="F250" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H250" t="s">
-        <v>834</v>
-      </c>
       <c r="I250" t="b">
         <v>1</v>
       </c>
       <c r="K250" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L250" t="s">
         <v>809</v>
@@ -10361,16 +10139,16 @@
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="B251" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="C251" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D251" s="5" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="E251" s="5" t="b">
         <v>0</v>
@@ -10378,14 +10156,11 @@
       <c r="F251" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H251" t="s">
-        <v>834</v>
-      </c>
       <c r="I251" t="b">
         <v>1</v>
       </c>
       <c r="K251" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L251" t="s">
         <v>809</v>
@@ -10393,16 +10168,16 @@
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="B252" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C252" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D252" s="5" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="E252" s="5" t="b">
         <v>0</v>
@@ -10410,14 +10185,11 @@
       <c r="F252" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H252" t="s">
-        <v>839</v>
-      </c>
       <c r="I252" t="b">
         <v>1</v>
       </c>
       <c r="K252" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L252" t="s">
         <v>809</v>
@@ -10425,16 +10197,16 @@
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="B253" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="C253" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D253" s="5" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="E253" s="5" t="b">
         <v>0</v>
@@ -10442,14 +10214,11 @@
       <c r="F253" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H253" t="s">
-        <v>814</v>
-      </c>
       <c r="I253" t="b">
         <v>1</v>
       </c>
       <c r="K253" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L253" t="s">
         <v>810</v>
@@ -10457,16 +10226,16 @@
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
-        <v>842</v>
+        <v>864</v>
       </c>
       <c r="B254" t="s">
-        <v>843</v>
+        <v>864</v>
       </c>
       <c r="C254" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D254" s="5" t="s">
-        <v>844</v>
+        <v>838</v>
       </c>
       <c r="E254" s="5" t="b">
         <v>0</v>
@@ -10474,31 +10243,28 @@
       <c r="F254" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H254" t="s">
-        <v>814</v>
-      </c>
       <c r="I254" t="b">
         <v>1</v>
       </c>
       <c r="K254" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L254" t="s">
-        <v>911</v>
+        <v>861</v>
       </c>
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>845</v>
+        <v>839</v>
       </c>
       <c r="B255" t="s">
-        <v>845</v>
+        <v>839</v>
       </c>
       <c r="C255" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D255" s="5" t="s">
-        <v>846</v>
+        <v>840</v>
       </c>
       <c r="E255" s="5" t="b">
         <v>0</v>
@@ -10506,14 +10272,11 @@
       <c r="F255" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H255" t="s">
-        <v>814</v>
-      </c>
       <c r="I255" t="b">
         <v>1</v>
       </c>
       <c r="K255" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L255" t="s">
         <v>809</v>
@@ -10521,16 +10284,16 @@
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>847</v>
+        <v>841</v>
       </c>
       <c r="B256" t="s">
-        <v>848</v>
+        <v>842</v>
       </c>
       <c r="C256" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D256" s="5" t="s">
-        <v>849</v>
+        <v>843</v>
       </c>
       <c r="E256" s="5" t="b">
         <v>0</v>
@@ -10538,14 +10301,11 @@
       <c r="F256" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H256" t="s">
-        <v>814</v>
-      </c>
       <c r="I256" t="b">
         <v>1</v>
       </c>
       <c r="K256" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L256" t="s">
         <v>811</v>
@@ -10553,16 +10313,16 @@
     </row>
     <row r="257" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>850</v>
+        <v>844</v>
       </c>
       <c r="B257" t="s">
-        <v>850</v>
+        <v>844</v>
       </c>
       <c r="C257" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D257" s="6" t="s">
-        <v>930</v>
+        <v>862</v>
       </c>
       <c r="E257" s="5" t="b">
         <v>0</v>
@@ -10570,14 +10330,11 @@
       <c r="F257" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H257" t="s">
-        <v>814</v>
-      </c>
       <c r="I257" t="b">
         <v>1</v>
       </c>
       <c r="K257" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L257" t="s">
         <v>809</v>
@@ -10585,16 +10342,16 @@
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>851</v>
+        <v>845</v>
       </c>
       <c r="B258" t="s">
-        <v>852</v>
+        <v>846</v>
       </c>
       <c r="C258" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D258" s="5" t="s">
-        <v>853</v>
+        <v>847</v>
       </c>
       <c r="E258" s="5" t="b">
         <v>0</v>
@@ -10602,14 +10359,11 @@
       <c r="F258" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H258" t="s">
-        <v>814</v>
-      </c>
       <c r="I258" t="b">
         <v>1</v>
       </c>
       <c r="K258" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L258" t="s">
         <v>809</v>
@@ -10617,16 +10371,16 @@
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="B259" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C259" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D259" s="5" t="s">
-        <v>855</v>
+        <v>849</v>
       </c>
       <c r="E259" s="5" t="b">
         <v>0</v>
@@ -10634,17 +10388,14 @@
       <c r="F259" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H259" t="s">
-        <v>814</v>
-      </c>
       <c r="I259" t="b">
         <v>1</v>
       </c>
       <c r="J259" t="s">
-        <v>856</v>
+        <v>850</v>
       </c>
       <c r="K259" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L259" t="s">
         <v>809</v>
@@ -10652,16 +10403,16 @@
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>857</v>
+        <v>851</v>
       </c>
       <c r="B260" t="s">
-        <v>857</v>
+        <v>851</v>
       </c>
       <c r="C260" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D260" s="5" t="s">
-        <v>858</v>
+        <v>852</v>
       </c>
       <c r="E260" s="5" t="b">
         <v>0</v>
@@ -10669,17 +10420,14 @@
       <c r="F260" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H260" t="s">
-        <v>814</v>
-      </c>
       <c r="I260" t="b">
         <v>1</v>
       </c>
       <c r="J260" t="s">
-        <v>859</v>
+        <v>853</v>
       </c>
       <c r="K260" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L260" t="s">
         <v>809</v>
@@ -10687,16 +10435,16 @@
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>860</v>
+        <v>854</v>
       </c>
       <c r="B261" t="s">
-        <v>860</v>
+        <v>854</v>
       </c>
       <c r="C261" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D261" s="5" t="s">
-        <v>861</v>
+        <v>855</v>
       </c>
       <c r="E261" s="5" t="b">
         <v>0</v>
@@ -10704,17 +10452,14 @@
       <c r="F261" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H261" t="s">
-        <v>814</v>
-      </c>
       <c r="I261" t="b">
         <v>1</v>
       </c>
       <c r="J261" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="K261" t="s">
-        <v>815</v>
+        <v>865</v>
       </c>
       <c r="L261" t="s">
         <v>809</v>
@@ -10722,668 +10467,142 @@
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>863</v>
+        <v>857</v>
       </c>
       <c r="B262" t="s">
-        <v>864</v>
+        <v>858</v>
       </c>
       <c r="C262" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D262" s="5" t="s">
+        <v>859</v>
+      </c>
+      <c r="E262" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F262" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I262" t="b">
+        <v>1</v>
+      </c>
+      <c r="J262" t="s">
+        <v>860</v>
+      </c>
+      <c r="K262" t="s">
         <v>865</v>
       </c>
-      <c r="E262" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F262" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H262" t="s">
-        <v>814</v>
-      </c>
-      <c r="I262" t="b">
-        <v>1</v>
-      </c>
-      <c r="J262" t="s">
-        <v>866</v>
-      </c>
-      <c r="K262" t="s">
-        <v>815</v>
-      </c>
       <c r="L262" t="s">
         <v>809</v>
       </c>
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A263" t="s">
-        <v>867</v>
-      </c>
-      <c r="B263" t="s">
-        <v>867</v>
-      </c>
-      <c r="C263" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D263" s="5" t="s">
-        <v>868</v>
-      </c>
-      <c r="E263" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F263" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H263" t="s">
-        <v>869</v>
-      </c>
-      <c r="I263" t="b">
-        <v>1</v>
-      </c>
-      <c r="J263" t="s">
-        <v>912</v>
-      </c>
-      <c r="K263" t="s">
-        <v>815</v>
-      </c>
-      <c r="L263" t="s">
-        <v>809</v>
-      </c>
+      <c r="C263" s="5"/>
+      <c r="D263" s="5"/>
+      <c r="E263" s="5"/>
+      <c r="F263" s="5"/>
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A264" t="s">
-        <v>870</v>
-      </c>
-      <c r="B264" t="s">
-        <v>871</v>
-      </c>
-      <c r="C264" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D264" s="5" t="s">
-        <v>872</v>
-      </c>
-      <c r="E264" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F264" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H264" t="s">
-        <v>869</v>
-      </c>
-      <c r="I264" t="b">
-        <v>1</v>
-      </c>
-      <c r="J264" t="s">
-        <v>913</v>
-      </c>
-      <c r="K264" t="s">
-        <v>815</v>
-      </c>
-      <c r="L264" t="s">
-        <v>809</v>
-      </c>
+      <c r="C264" s="5"/>
+      <c r="D264" s="5"/>
+      <c r="E264" s="5"/>
+      <c r="F264" s="5"/>
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A265" t="s">
-        <v>873</v>
-      </c>
-      <c r="B265" t="s">
-        <v>873</v>
-      </c>
-      <c r="C265" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D265" s="5" t="s">
-        <v>874</v>
-      </c>
-      <c r="E265" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F265" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H265" t="s">
-        <v>869</v>
-      </c>
-      <c r="I265" t="b">
-        <v>1</v>
-      </c>
-      <c r="J265" t="s">
-        <v>914</v>
-      </c>
-      <c r="K265" t="s">
-        <v>815</v>
-      </c>
-      <c r="L265" t="s">
-        <v>809</v>
-      </c>
+      <c r="C265" s="5"/>
+      <c r="D265" s="5"/>
+      <c r="E265" s="5"/>
+      <c r="F265" s="5"/>
     </row>
     <row r="266" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A266" t="s">
-        <v>875</v>
-      </c>
-      <c r="B266" t="s">
-        <v>876</v>
-      </c>
-      <c r="C266" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D266" s="5" t="s">
-        <v>877</v>
-      </c>
-      <c r="E266" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F266" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H266" t="s">
-        <v>869</v>
-      </c>
-      <c r="I266" t="b">
-        <v>1</v>
-      </c>
-      <c r="J266" t="s">
-        <v>915</v>
-      </c>
-      <c r="K266" t="s">
-        <v>815</v>
-      </c>
-      <c r="L266" t="s">
-        <v>809</v>
-      </c>
+      <c r="C266" s="5"/>
+      <c r="D266" s="5"/>
+      <c r="E266" s="5"/>
+      <c r="F266" s="5"/>
     </row>
     <row r="267" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A267" t="s">
-        <v>418</v>
-      </c>
-      <c r="B267" t="s">
-        <v>563</v>
-      </c>
-      <c r="C267" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D267" s="5" t="s">
-        <v>878</v>
-      </c>
-      <c r="E267" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F267" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H267" t="s">
-        <v>869</v>
-      </c>
-      <c r="I267" t="b">
-        <v>1</v>
-      </c>
-      <c r="J267" t="s">
-        <v>916</v>
-      </c>
-      <c r="K267" t="s">
-        <v>815</v>
-      </c>
-      <c r="L267" t="s">
-        <v>809</v>
-      </c>
+      <c r="C267" s="5"/>
+      <c r="D267" s="5"/>
+      <c r="E267" s="5"/>
+      <c r="F267" s="5"/>
     </row>
     <row r="268" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A268" s="2" t="s">
-        <v>879</v>
-      </c>
-      <c r="B268" t="s">
-        <v>880</v>
-      </c>
-      <c r="C268" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D268" s="5" t="s">
-        <v>881</v>
-      </c>
-      <c r="E268" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F268" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H268" t="s">
-        <v>869</v>
-      </c>
-      <c r="I268" t="b">
-        <v>1</v>
-      </c>
-      <c r="J268" t="s">
-        <v>917</v>
-      </c>
-      <c r="K268" t="s">
-        <v>815</v>
-      </c>
-      <c r="L268" t="s">
-        <v>809</v>
-      </c>
+      <c r="A268" s="2"/>
+      <c r="C268" s="5"/>
+      <c r="D268" s="5"/>
+      <c r="E268" s="5"/>
+      <c r="F268" s="5"/>
     </row>
     <row r="269" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A269" t="s">
-        <v>882</v>
-      </c>
-      <c r="B269" t="s">
-        <v>882</v>
-      </c>
-      <c r="C269" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D269" s="5" t="s">
-        <v>883</v>
-      </c>
-      <c r="E269" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F269" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H269" t="s">
-        <v>869</v>
-      </c>
-      <c r="I269" t="b">
-        <v>1</v>
-      </c>
-      <c r="J269" t="s">
-        <v>918</v>
-      </c>
-      <c r="K269" t="s">
-        <v>815</v>
-      </c>
-      <c r="L269" t="s">
-        <v>809</v>
-      </c>
+      <c r="C269" s="5"/>
+      <c r="D269" s="5"/>
+      <c r="E269" s="5"/>
+      <c r="F269" s="5"/>
     </row>
     <row r="270" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A270" t="s">
-        <v>884</v>
-      </c>
-      <c r="B270" t="s">
-        <v>885</v>
-      </c>
-      <c r="C270" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D270" s="5" t="s">
-        <v>886</v>
-      </c>
-      <c r="E270" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F270" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H270" t="s">
-        <v>869</v>
-      </c>
-      <c r="I270" t="b">
-        <v>1</v>
-      </c>
-      <c r="J270" t="s">
-        <v>919</v>
-      </c>
-      <c r="K270" t="s">
-        <v>815</v>
-      </c>
-      <c r="L270" t="s">
-        <v>809</v>
-      </c>
+      <c r="C270" s="5"/>
+      <c r="D270" s="5"/>
+      <c r="E270" s="5"/>
+      <c r="F270" s="5"/>
     </row>
     <row r="271" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A271" t="s">
-        <v>887</v>
-      </c>
-      <c r="B271" t="s">
-        <v>887</v>
-      </c>
-      <c r="C271" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D271" s="5" t="s">
-        <v>888</v>
-      </c>
-      <c r="E271" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F271" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H271" t="s">
-        <v>869</v>
-      </c>
-      <c r="I271" t="b">
-        <v>1</v>
-      </c>
-      <c r="J271" t="s">
-        <v>920</v>
-      </c>
-      <c r="K271" t="s">
-        <v>815</v>
-      </c>
-      <c r="L271" t="s">
-        <v>810</v>
-      </c>
+      <c r="C271" s="5"/>
+      <c r="D271" s="5"/>
+      <c r="E271" s="5"/>
+      <c r="F271" s="5"/>
     </row>
     <row r="272" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A272" t="s">
-        <v>889</v>
-      </c>
-      <c r="B272" t="s">
-        <v>889</v>
-      </c>
-      <c r="C272" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D272" s="5" t="s">
-        <v>890</v>
-      </c>
-      <c r="E272" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F272" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H272" t="s">
-        <v>869</v>
-      </c>
-      <c r="I272" t="b">
-        <v>1</v>
-      </c>
-      <c r="J272" t="s">
-        <v>921</v>
-      </c>
-      <c r="K272" t="s">
-        <v>815</v>
-      </c>
-      <c r="L272" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A273" t="s">
-        <v>891</v>
-      </c>
-      <c r="B273" t="s">
-        <v>891</v>
-      </c>
-      <c r="C273" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D273" s="5" t="s">
-        <v>892</v>
-      </c>
-      <c r="E273" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F273" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H273" t="s">
-        <v>893</v>
-      </c>
-      <c r="I273" t="b">
-        <v>1</v>
-      </c>
-      <c r="J273" t="s">
-        <v>922</v>
-      </c>
-      <c r="K273" t="s">
-        <v>815</v>
-      </c>
-      <c r="L273" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A274" t="s">
-        <v>894</v>
-      </c>
-      <c r="B274" t="s">
-        <v>894</v>
-      </c>
-      <c r="C274" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D274" s="5" t="s">
-        <v>895</v>
-      </c>
-      <c r="E274" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F274" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H274" t="s">
-        <v>869</v>
-      </c>
-      <c r="I274" t="b">
-        <v>1</v>
-      </c>
-      <c r="J274" t="s">
-        <v>923</v>
-      </c>
-      <c r="K274" t="s">
-        <v>815</v>
-      </c>
-      <c r="L274" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A275" t="s">
-        <v>896</v>
-      </c>
-      <c r="B275" t="s">
-        <v>896</v>
-      </c>
-      <c r="C275" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D275" s="5" t="s">
-        <v>897</v>
-      </c>
-      <c r="E275" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F275" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H275" t="s">
-        <v>869</v>
-      </c>
-      <c r="I275" t="b">
-        <v>1</v>
-      </c>
-      <c r="J275" t="s">
-        <v>924</v>
-      </c>
-      <c r="K275" t="s">
-        <v>815</v>
-      </c>
-      <c r="L275" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A276" t="s">
-        <v>898</v>
-      </c>
-      <c r="B276" t="s">
-        <v>898</v>
-      </c>
-      <c r="C276" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D276" s="5" t="s">
-        <v>899</v>
-      </c>
-      <c r="E276" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F276" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H276" t="s">
-        <v>869</v>
-      </c>
-      <c r="I276" t="b">
-        <v>1</v>
-      </c>
-      <c r="J276" t="s">
-        <v>925</v>
-      </c>
-      <c r="K276" t="s">
-        <v>815</v>
-      </c>
-      <c r="L276" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A277" t="s">
-        <v>900</v>
-      </c>
-      <c r="B277" t="s">
-        <v>900</v>
-      </c>
-      <c r="C277" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D277" s="5" t="s">
-        <v>901</v>
-      </c>
-      <c r="E277" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F277" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H277" t="s">
-        <v>869</v>
-      </c>
-      <c r="I277" t="b">
-        <v>1</v>
-      </c>
-      <c r="J277" t="s">
-        <v>926</v>
-      </c>
-      <c r="K277" t="s">
-        <v>815</v>
-      </c>
-      <c r="L277" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A278" t="s">
-        <v>902</v>
-      </c>
-      <c r="B278" t="s">
-        <v>902</v>
-      </c>
-      <c r="C278" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D278" s="5" t="s">
-        <v>903</v>
-      </c>
-      <c r="E278" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F278" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H278" t="s">
-        <v>869</v>
-      </c>
-      <c r="I278" t="b">
-        <v>1</v>
-      </c>
-      <c r="J278" t="s">
-        <v>927</v>
-      </c>
-      <c r="K278" t="s">
-        <v>815</v>
-      </c>
-      <c r="L278" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A279" t="s">
-        <v>904</v>
-      </c>
-      <c r="B279" t="s">
-        <v>905</v>
-      </c>
-      <c r="C279" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D279" t="s">
-        <v>906</v>
-      </c>
-      <c r="E279" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F279" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H279" t="s">
-        <v>907</v>
-      </c>
-      <c r="I279" t="b">
-        <v>1</v>
-      </c>
-      <c r="J279" t="s">
-        <v>928</v>
-      </c>
-      <c r="K279" t="s">
-        <v>815</v>
-      </c>
-      <c r="L279" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A280" t="s">
-        <v>908</v>
-      </c>
-      <c r="B280" t="s">
-        <v>909</v>
-      </c>
-      <c r="C280" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D280" t="s">
-        <v>910</v>
-      </c>
-      <c r="E280" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F280" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H280" t="s">
-        <v>893</v>
-      </c>
-      <c r="I280" t="b">
-        <v>1</v>
-      </c>
-      <c r="J280" t="s">
-        <v>929</v>
-      </c>
-      <c r="K280" t="s">
-        <v>815</v>
-      </c>
-      <c r="L280" t="s">
-        <v>809</v>
-      </c>
+      <c r="C272" s="5"/>
+      <c r="D272" s="5"/>
+      <c r="E272" s="5"/>
+      <c r="F272" s="5"/>
+    </row>
+    <row r="273" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C273" s="5"/>
+      <c r="D273" s="5"/>
+      <c r="E273" s="5"/>
+      <c r="F273" s="5"/>
+    </row>
+    <row r="274" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C274" s="5"/>
+      <c r="D274" s="5"/>
+      <c r="E274" s="5"/>
+      <c r="F274" s="5"/>
+    </row>
+    <row r="275" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C275" s="5"/>
+      <c r="D275" s="5"/>
+      <c r="E275" s="5"/>
+      <c r="F275" s="5"/>
+    </row>
+    <row r="276" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C276" s="5"/>
+      <c r="D276" s="5"/>
+      <c r="E276" s="5"/>
+      <c r="F276" s="5"/>
+    </row>
+    <row r="277" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C277" s="5"/>
+      <c r="D277" s="5"/>
+      <c r="E277" s="5"/>
+      <c r="F277" s="5"/>
+    </row>
+    <row r="278" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C278" s="5"/>
+      <c r="D278" s="5"/>
+      <c r="E278" s="5"/>
+      <c r="F278" s="5"/>
+    </row>
+    <row r="279" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C279" s="5"/>
+      <c r="E279" s="5"/>
+      <c r="F279" s="5"/>
+    </row>
+    <row r="280" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C280" s="5"/>
+      <c r="E280" s="5"/>
+      <c r="F280" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new build new breakdowns
</commit_message>
<xml_diff>
--- a/data/compleat_wiki_man.xlsx
+++ b/data/compleat_wiki_man.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe\Documents\GitHub\PhyrexianDictionary\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93783722-7449-4E98-8904-8E51DC33AF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9021E91E-42A3-4666-A414-BCC94C01CDB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2006" uniqueCount="929">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="865">
   <si>
     <t>IPA</t>
   </si>
@@ -2459,12 +2459,6 @@
     <t>Indicative, Present</t>
   </si>
   <si>
-    <t>mood</t>
-  </si>
-  <si>
-    <t>particle</t>
-  </si>
-  <si>
     <t>'u</t>
   </si>
   <si>
@@ -2519,9 +2513,6 @@
     <t>Alternative (or)</t>
   </si>
   <si>
-    <t>mood, suffix</t>
-  </si>
-  <si>
     <t>xə</t>
   </si>
   <si>
@@ -2534,9 +2525,6 @@
     <t>Negative (un-, not)</t>
   </si>
   <si>
-    <t>mood, prefix</t>
-  </si>
-  <si>
     <t>əl</t>
   </si>
   <si>
@@ -2618,195 +2606,9 @@
     <t>Paired with past</t>
   </si>
   <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>to (spatial)</t>
-  </si>
-  <si>
-    <t>prefix</t>
-  </si>
-  <si>
-    <t>əšq</t>
-  </si>
-  <si>
-    <t>əʃq</t>
-  </si>
-  <si>
-    <t>on (spatial)</t>
-  </si>
-  <si>
-    <t>dl</t>
-  </si>
-  <si>
-    <t>in (spatial)</t>
-  </si>
-  <si>
-    <t>φɒ'</t>
-  </si>
-  <si>
-    <t>φɒʔ</t>
-  </si>
-  <si>
-    <t>until (temporal)</t>
-  </si>
-  <si>
-    <t>for (temporal)</t>
-  </si>
-  <si>
-    <t>'ɒp</t>
-  </si>
-  <si>
-    <t>ʔɒp</t>
-  </si>
-  <si>
-    <t>any</t>
-  </si>
-  <si>
-    <t>ɢə</t>
-  </si>
-  <si>
-    <t>this/that</t>
-  </si>
-  <si>
-    <t>ɣẅ</t>
-  </si>
-  <si>
-    <t>ɣɯ</t>
-  </si>
-  <si>
-    <t>from</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>of</t>
-  </si>
-  <si>
-    <t>qər</t>
-  </si>
-  <si>
-    <t>with</t>
-  </si>
-  <si>
-    <t>gr</t>
-  </si>
-  <si>
-    <t>than</t>
-  </si>
-  <si>
-    <t>prefix, suffix</t>
-  </si>
-  <si>
-    <t>pl</t>
-  </si>
-  <si>
-    <t>completion</t>
-  </si>
-  <si>
-    <t>plθ</t>
-  </si>
-  <si>
-    <t>not-completion</t>
-  </si>
-  <si>
-    <t>pn</t>
-  </si>
-  <si>
-    <t>greater</t>
-  </si>
-  <si>
-    <t>ke</t>
-  </si>
-  <si>
-    <t>collective</t>
-  </si>
-  <si>
-    <t>ɣwi</t>
-  </si>
-  <si>
-    <t>ability</t>
-  </si>
-  <si>
-    <t>tč</t>
-  </si>
-  <si>
-    <t>ttʃ</t>
-  </si>
-  <si>
-    <t>indicate order</t>
-  </si>
-  <si>
-    <t>suffix</t>
-  </si>
-  <si>
-    <t>xe_'ə</t>
-  </si>
-  <si>
-    <t>xe_ʔə</t>
-  </si>
-  <si>
-    <t>indicate frequency</t>
-  </si>
-  <si>
     <t>poor</t>
   </si>
   <si>
-    <t>'return this to your hand'</t>
-  </si>
-  <si>
-    <t>'put a counter on this'</t>
-  </si>
-  <si>
-    <t>'target card in your graveyard'</t>
-  </si>
-  <si>
-    <t>'until your next turn'</t>
-  </si>
-  <si>
-    <t>'you can do this for this turn'</t>
-  </si>
-  <si>
-    <t>'produce mana of any type'</t>
-  </si>
-  <si>
-    <t>'sacrifice this creature'</t>
-  </si>
-  <si>
-    <t>'a card from your deck'</t>
-  </si>
-  <si>
-    <t>'ability of a permanent'</t>
-  </si>
-  <si>
-    <t>'destroy all permanents with counters'</t>
-  </si>
-  <si>
-    <t>'more/less than'</t>
-  </si>
-  <si>
-    <t>'Complete (prefix + make)'</t>
-  </si>
-  <si>
-    <t>'half, rounded down (prefix + not + two + amounts)'</t>
-  </si>
-  <si>
-    <t>'Vigilance (ability + prefix + see)'</t>
-  </si>
-  <si>
-    <t>'world (prefix + land)'</t>
-  </si>
-  <si>
-    <t>'Immortality (prefix + un + death)'</t>
-  </si>
-  <si>
-    <t>Number-related. 'Top (first) card of your library '</t>
-  </si>
-  <si>
-    <t>Number-related. 'once per turn'</t>
-  </si>
-  <si>
     <t>'Unless'</t>
   </si>
   <si>
@@ -2820,6 +2622,12 @@
   </si>
   <si>
     <t>vuwk</t>
+  </si>
+  <si>
+    <t>marker</t>
+  </si>
+  <si>
+    <t>number</t>
   </si>
 </sst>
 </file>
@@ -3218,10 +3026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L279"/>
+  <dimension ref="A1:L261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="M113" sqref="M113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5375,7 +5183,7 @@
         <v>628</v>
       </c>
       <c r="D76" t="s">
-        <v>925</v>
+        <v>859</v>
       </c>
       <c r="E76" t="s">
         <v>294</v>
@@ -5998,10 +5806,10 @@
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>926</v>
+        <v>860</v>
       </c>
       <c r="B98" t="s">
-        <v>926</v>
+        <v>860</v>
       </c>
       <c r="C98" t="b">
         <v>0</v>
@@ -6010,7 +5818,7 @@
         <v>93</v>
       </c>
       <c r="E98" t="s">
-        <v>926</v>
+        <v>860</v>
       </c>
       <c r="H98" t="s">
         <v>603</v>
@@ -6359,7 +6167,7 @@
         <v>1</v>
       </c>
       <c r="K110" t="s">
-        <v>576</v>
+        <v>864</v>
       </c>
       <c r="L110" t="s">
         <v>803</v>
@@ -6388,7 +6196,7 @@
         <v>1</v>
       </c>
       <c r="K111" t="s">
-        <v>576</v>
+        <v>864</v>
       </c>
       <c r="L111" t="s">
         <v>803</v>
@@ -6417,7 +6225,7 @@
         <v>1</v>
       </c>
       <c r="K112" t="s">
-        <v>576</v>
+        <v>864</v>
       </c>
       <c r="L112" t="s">
         <v>803</v>
@@ -8129,7 +7937,7 @@
         <v>660</v>
       </c>
       <c r="D173" t="s">
-        <v>927</v>
+        <v>861</v>
       </c>
       <c r="E173" t="s">
         <v>2</v>
@@ -8233,10 +8041,10 @@
     </row>
     <row r="177" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>928</v>
+        <v>862</v>
       </c>
       <c r="B177" t="s">
-        <v>928</v>
+        <v>862</v>
       </c>
       <c r="C177" t="b">
         <v>0</v>
@@ -8245,7 +8053,7 @@
         <v>169</v>
       </c>
       <c r="E177" t="s">
-        <v>928</v>
+        <v>862</v>
       </c>
       <c r="H177" t="s">
         <v>603</v>
@@ -10055,14 +9863,11 @@
       <c r="F241" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H241" t="s">
-        <v>808</v>
-      </c>
       <c r="I241" t="b">
         <v>1</v>
       </c>
       <c r="K241" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L241" t="s">
         <v>803</v>
@@ -10070,31 +9875,28 @@
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="B242" t="s">
+        <v>809</v>
+      </c>
+      <c r="C242" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D242" s="5" t="s">
         <v>810</v>
       </c>
-      <c r="B242" t="s">
-        <v>811</v>
-      </c>
-      <c r="C242" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D242" s="5" t="s">
-        <v>812</v>
-      </c>
       <c r="E242" s="5" t="b">
         <v>0</v>
       </c>
       <c r="F242" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H242" t="s">
-        <v>808</v>
-      </c>
       <c r="I242" t="b">
         <v>1</v>
       </c>
       <c r="K242" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L242" t="s">
         <v>803</v>
@@ -10102,16 +9904,16 @@
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B243" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="C243" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D243" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="E243" s="5" t="b">
         <v>0</v>
@@ -10119,14 +9921,11 @@
       <c r="F243" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H243" t="s">
-        <v>808</v>
-      </c>
       <c r="I243" t="b">
         <v>1</v>
       </c>
       <c r="K243" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L243" t="s">
         <v>803</v>
@@ -10134,31 +9933,28 @@
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
+        <v>813</v>
+      </c>
+      <c r="B244" t="s">
+        <v>814</v>
+      </c>
+      <c r="C244" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D244" s="5" t="s">
         <v>815</v>
       </c>
-      <c r="B244" t="s">
-        <v>816</v>
-      </c>
-      <c r="C244" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D244" s="5" t="s">
-        <v>817</v>
-      </c>
       <c r="E244" s="5" t="b">
         <v>0</v>
       </c>
       <c r="F244" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H244" t="s">
-        <v>808</v>
-      </c>
       <c r="I244" t="b">
         <v>1</v>
       </c>
       <c r="K244" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L244" t="s">
         <v>803</v>
@@ -10166,16 +9962,16 @@
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="B245" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C245" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D245" s="5" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="E245" s="5" t="b">
         <v>0</v>
@@ -10183,14 +9979,11 @@
       <c r="F245" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H245" t="s">
-        <v>808</v>
-      </c>
       <c r="I245" t="b">
         <v>1</v>
       </c>
       <c r="K245" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L245" t="s">
         <v>803</v>
@@ -10198,16 +9991,16 @@
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B246" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="C246" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D246" s="5" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E246" s="5" t="b">
         <v>0</v>
@@ -10215,14 +10008,11 @@
       <c r="F246" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H246" t="s">
-        <v>808</v>
-      </c>
       <c r="I246" t="b">
         <v>1</v>
       </c>
       <c r="K246" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L246" t="s">
         <v>803</v>
@@ -10230,16 +10020,16 @@
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="B247" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="C247" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D247" s="5" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="E247" s="5" t="b">
         <v>0</v>
@@ -10247,14 +10037,11 @@
       <c r="F247" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H247" t="s">
-        <v>808</v>
-      </c>
       <c r="I247" t="b">
         <v>1</v>
       </c>
       <c r="K247" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L247" t="s">
         <v>803</v>
@@ -10262,16 +10049,16 @@
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B248" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="C248" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D248" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="E248" s="5" t="b">
         <v>0</v>
@@ -10279,14 +10066,11 @@
       <c r="F248" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H248" t="s">
-        <v>808</v>
-      </c>
       <c r="I248" t="b">
         <v>1</v>
       </c>
       <c r="K248" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L248" t="s">
         <v>803</v>
@@ -10294,16 +10078,16 @@
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B249" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="C249" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D249" s="5" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="E249" s="5" t="b">
         <v>0</v>
@@ -10311,14 +10095,11 @@
       <c r="F249" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H249" t="s">
-        <v>828</v>
-      </c>
       <c r="I249" t="b">
         <v>1</v>
       </c>
       <c r="K249" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L249" t="s">
         <v>803</v>
@@ -10326,16 +10107,16 @@
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="B250" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="C250" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D250" s="5" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="E250" s="5" t="b">
         <v>0</v>
@@ -10343,14 +10124,11 @@
       <c r="F250" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H250" t="s">
-        <v>828</v>
-      </c>
       <c r="I250" t="b">
         <v>1</v>
       </c>
       <c r="K250" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L250" t="s">
         <v>803</v>
@@ -10358,16 +10136,16 @@
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="B251" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="C251" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D251" s="5" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="E251" s="5" t="b">
         <v>0</v>
@@ -10375,14 +10153,11 @@
       <c r="F251" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H251" t="s">
-        <v>833</v>
-      </c>
       <c r="I251" t="b">
         <v>1</v>
       </c>
       <c r="K251" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L251" t="s">
         <v>803</v>
@@ -10390,16 +10165,16 @@
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="B252" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="C252" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D252" s="5" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="E252" s="5" t="b">
         <v>0</v>
@@ -10407,14 +10182,11 @@
       <c r="F252" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H252" t="s">
-        <v>808</v>
-      </c>
       <c r="I252" t="b">
         <v>1</v>
       </c>
       <c r="K252" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L252" t="s">
         <v>804</v>
@@ -10422,16 +10194,16 @@
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="B253" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="C253" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D253" s="5" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="E253" s="5" t="b">
         <v>0</v>
@@ -10439,31 +10211,28 @@
       <c r="F253" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H253" t="s">
-        <v>808</v>
-      </c>
       <c r="I253" t="b">
         <v>1</v>
       </c>
       <c r="K253" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L253" t="s">
-        <v>905</v>
+        <v>857</v>
       </c>
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="B254" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="C254" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D254" s="5" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="E254" s="5" t="b">
         <v>0</v>
@@ -10471,14 +10240,11 @@
       <c r="F254" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H254" t="s">
-        <v>808</v>
-      </c>
       <c r="I254" t="b">
         <v>1</v>
       </c>
       <c r="K254" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L254" t="s">
         <v>803</v>
@@ -10486,16 +10252,16 @@
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="B255" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="C255" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D255" s="5" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="E255" s="5" t="b">
         <v>0</v>
@@ -10503,14 +10269,11 @@
       <c r="F255" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H255" t="s">
-        <v>808</v>
-      </c>
       <c r="I255" t="b">
         <v>1</v>
       </c>
       <c r="K255" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L255" t="s">
         <v>805</v>
@@ -10518,16 +10281,16 @@
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="B256" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="C256" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D256" s="6" t="s">
-        <v>924</v>
+        <v>858</v>
       </c>
       <c r="E256" s="5" t="b">
         <v>0</v>
@@ -10535,14 +10298,11 @@
       <c r="F256" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H256" t="s">
-        <v>808</v>
-      </c>
       <c r="I256" t="b">
         <v>1</v>
       </c>
       <c r="K256" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L256" t="s">
         <v>803</v>
@@ -10550,16 +10310,16 @@
     </row>
     <row r="257" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>845</v>
+        <v>841</v>
       </c>
       <c r="B257" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
       <c r="C257" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D257" s="5" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
       <c r="E257" s="5" t="b">
         <v>0</v>
@@ -10567,14 +10327,11 @@
       <c r="F257" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H257" t="s">
-        <v>808</v>
-      </c>
       <c r="I257" t="b">
         <v>1</v>
       </c>
       <c r="K257" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L257" t="s">
         <v>803</v>
@@ -10582,16 +10339,16 @@
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="B258" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="C258" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D258" s="5" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="E258" s="5" t="b">
         <v>0</v>
@@ -10599,17 +10356,14 @@
       <c r="F258" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H258" t="s">
-        <v>808</v>
-      </c>
       <c r="I258" t="b">
         <v>1</v>
       </c>
       <c r="J258" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="K258" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L258" t="s">
         <v>803</v>
@@ -10617,16 +10371,16 @@
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="B259" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="C259" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D259" s="5" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="E259" s="5" t="b">
         <v>0</v>
@@ -10634,17 +10388,14 @@
       <c r="F259" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H259" t="s">
-        <v>808</v>
-      </c>
       <c r="I259" t="b">
         <v>1</v>
       </c>
       <c r="J259" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="K259" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L259" t="s">
         <v>803</v>
@@ -10652,16 +10403,16 @@
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="B260" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="C260" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D260" s="5" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="E260" s="5" t="b">
         <v>0</v>
@@ -10669,17 +10420,14 @@
       <c r="F260" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H260" t="s">
-        <v>808</v>
-      </c>
       <c r="I260" t="b">
         <v>1</v>
       </c>
       <c r="J260" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="K260" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L260" t="s">
         <v>803</v>
@@ -10687,16 +10435,16 @@
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="B261" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="C261" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D261" s="5" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="E261" s="5" t="b">
         <v>0</v>
@@ -10704,649 +10452,16 @@
       <c r="F261" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H261" t="s">
-        <v>808</v>
-      </c>
       <c r="I261" t="b">
         <v>1</v>
       </c>
       <c r="J261" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="K261" t="s">
-        <v>809</v>
+        <v>863</v>
       </c>
       <c r="L261" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A262" t="s">
-        <v>861</v>
-      </c>
-      <c r="B262" t="s">
-        <v>861</v>
-      </c>
-      <c r="C262" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D262" s="5" t="s">
-        <v>862</v>
-      </c>
-      <c r="E262" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F262" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H262" t="s">
-        <v>863</v>
-      </c>
-      <c r="I262" t="b">
-        <v>1</v>
-      </c>
-      <c r="J262" t="s">
-        <v>906</v>
-      </c>
-      <c r="K262" t="s">
-        <v>809</v>
-      </c>
-      <c r="L262" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A263" t="s">
-        <v>864</v>
-      </c>
-      <c r="B263" t="s">
-        <v>865</v>
-      </c>
-      <c r="C263" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D263" s="5" t="s">
-        <v>866</v>
-      </c>
-      <c r="E263" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F263" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H263" t="s">
-        <v>863</v>
-      </c>
-      <c r="I263" t="b">
-        <v>1</v>
-      </c>
-      <c r="J263" t="s">
-        <v>907</v>
-      </c>
-      <c r="K263" t="s">
-        <v>809</v>
-      </c>
-      <c r="L263" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A264" t="s">
-        <v>867</v>
-      </c>
-      <c r="B264" t="s">
-        <v>867</v>
-      </c>
-      <c r="C264" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D264" s="5" t="s">
-        <v>868</v>
-      </c>
-      <c r="E264" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F264" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H264" t="s">
-        <v>863</v>
-      </c>
-      <c r="I264" t="b">
-        <v>1</v>
-      </c>
-      <c r="J264" t="s">
-        <v>908</v>
-      </c>
-      <c r="K264" t="s">
-        <v>809</v>
-      </c>
-      <c r="L264" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A265" t="s">
-        <v>869</v>
-      </c>
-      <c r="B265" t="s">
-        <v>870</v>
-      </c>
-      <c r="C265" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D265" s="5" t="s">
-        <v>871</v>
-      </c>
-      <c r="E265" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F265" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H265" t="s">
-        <v>863</v>
-      </c>
-      <c r="I265" t="b">
-        <v>1</v>
-      </c>
-      <c r="J265" t="s">
-        <v>909</v>
-      </c>
-      <c r="K265" t="s">
-        <v>809</v>
-      </c>
-      <c r="L265" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A266" t="s">
-        <v>415</v>
-      </c>
-      <c r="B266" t="s">
-        <v>558</v>
-      </c>
-      <c r="C266" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D266" s="5" t="s">
-        <v>872</v>
-      </c>
-      <c r="E266" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F266" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H266" t="s">
-        <v>863</v>
-      </c>
-      <c r="I266" t="b">
-        <v>1</v>
-      </c>
-      <c r="J266" t="s">
-        <v>910</v>
-      </c>
-      <c r="K266" t="s">
-        <v>809</v>
-      </c>
-      <c r="L266" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A267" s="2" t="s">
-        <v>873</v>
-      </c>
-      <c r="B267" t="s">
-        <v>874</v>
-      </c>
-      <c r="C267" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D267" s="5" t="s">
-        <v>875</v>
-      </c>
-      <c r="E267" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F267" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H267" t="s">
-        <v>863</v>
-      </c>
-      <c r="I267" t="b">
-        <v>1</v>
-      </c>
-      <c r="J267" t="s">
-        <v>911</v>
-      </c>
-      <c r="K267" t="s">
-        <v>809</v>
-      </c>
-      <c r="L267" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A268" t="s">
-        <v>876</v>
-      </c>
-      <c r="B268" t="s">
-        <v>876</v>
-      </c>
-      <c r="C268" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D268" s="5" t="s">
-        <v>877</v>
-      </c>
-      <c r="E268" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F268" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H268" t="s">
-        <v>863</v>
-      </c>
-      <c r="I268" t="b">
-        <v>1</v>
-      </c>
-      <c r="J268" t="s">
-        <v>912</v>
-      </c>
-      <c r="K268" t="s">
-        <v>809</v>
-      </c>
-      <c r="L268" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A269" t="s">
-        <v>878</v>
-      </c>
-      <c r="B269" t="s">
-        <v>879</v>
-      </c>
-      <c r="C269" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D269" s="5" t="s">
-        <v>880</v>
-      </c>
-      <c r="E269" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F269" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H269" t="s">
-        <v>863</v>
-      </c>
-      <c r="I269" t="b">
-        <v>1</v>
-      </c>
-      <c r="J269" t="s">
-        <v>913</v>
-      </c>
-      <c r="K269" t="s">
-        <v>809</v>
-      </c>
-      <c r="L269" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A270" t="s">
-        <v>881</v>
-      </c>
-      <c r="B270" t="s">
-        <v>881</v>
-      </c>
-      <c r="C270" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D270" s="5" t="s">
-        <v>882</v>
-      </c>
-      <c r="E270" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F270" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H270" t="s">
-        <v>863</v>
-      </c>
-      <c r="I270" t="b">
-        <v>1</v>
-      </c>
-      <c r="J270" t="s">
-        <v>914</v>
-      </c>
-      <c r="K270" t="s">
-        <v>809</v>
-      </c>
-      <c r="L270" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A271" t="s">
-        <v>883</v>
-      </c>
-      <c r="B271" t="s">
-        <v>883</v>
-      </c>
-      <c r="C271" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D271" s="5" t="s">
-        <v>884</v>
-      </c>
-      <c r="E271" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F271" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H271" t="s">
-        <v>863</v>
-      </c>
-      <c r="I271" t="b">
-        <v>1</v>
-      </c>
-      <c r="J271" t="s">
-        <v>915</v>
-      </c>
-      <c r="K271" t="s">
-        <v>809</v>
-      </c>
-      <c r="L271" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A272" t="s">
-        <v>885</v>
-      </c>
-      <c r="B272" t="s">
-        <v>885</v>
-      </c>
-      <c r="C272" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D272" s="5" t="s">
-        <v>886</v>
-      </c>
-      <c r="E272" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F272" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H272" t="s">
-        <v>887</v>
-      </c>
-      <c r="I272" t="b">
-        <v>1</v>
-      </c>
-      <c r="J272" t="s">
-        <v>916</v>
-      </c>
-      <c r="K272" t="s">
-        <v>809</v>
-      </c>
-      <c r="L272" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A273" t="s">
-        <v>888</v>
-      </c>
-      <c r="B273" t="s">
-        <v>888</v>
-      </c>
-      <c r="C273" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D273" s="5" t="s">
-        <v>889</v>
-      </c>
-      <c r="E273" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F273" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H273" t="s">
-        <v>863</v>
-      </c>
-      <c r="I273" t="b">
-        <v>1</v>
-      </c>
-      <c r="J273" t="s">
-        <v>917</v>
-      </c>
-      <c r="K273" t="s">
-        <v>809</v>
-      </c>
-      <c r="L273" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A274" t="s">
-        <v>890</v>
-      </c>
-      <c r="B274" t="s">
-        <v>890</v>
-      </c>
-      <c r="C274" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D274" s="5" t="s">
-        <v>891</v>
-      </c>
-      <c r="E274" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F274" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H274" t="s">
-        <v>863</v>
-      </c>
-      <c r="I274" t="b">
-        <v>1</v>
-      </c>
-      <c r="J274" t="s">
-        <v>918</v>
-      </c>
-      <c r="K274" t="s">
-        <v>809</v>
-      </c>
-      <c r="L274" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A275" t="s">
-        <v>892</v>
-      </c>
-      <c r="B275" t="s">
-        <v>892</v>
-      </c>
-      <c r="C275" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D275" s="5" t="s">
-        <v>893</v>
-      </c>
-      <c r="E275" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F275" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H275" t="s">
-        <v>863</v>
-      </c>
-      <c r="I275" t="b">
-        <v>1</v>
-      </c>
-      <c r="J275" t="s">
-        <v>919</v>
-      </c>
-      <c r="K275" t="s">
-        <v>809</v>
-      </c>
-      <c r="L275" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A276" t="s">
-        <v>894</v>
-      </c>
-      <c r="B276" t="s">
-        <v>894</v>
-      </c>
-      <c r="C276" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D276" s="5" t="s">
-        <v>895</v>
-      </c>
-      <c r="E276" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F276" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H276" t="s">
-        <v>863</v>
-      </c>
-      <c r="I276" t="b">
-        <v>1</v>
-      </c>
-      <c r="J276" t="s">
-        <v>920</v>
-      </c>
-      <c r="K276" t="s">
-        <v>809</v>
-      </c>
-      <c r="L276" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A277" t="s">
-        <v>896</v>
-      </c>
-      <c r="B277" t="s">
-        <v>896</v>
-      </c>
-      <c r="C277" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D277" s="5" t="s">
-        <v>897</v>
-      </c>
-      <c r="E277" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F277" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H277" t="s">
-        <v>863</v>
-      </c>
-      <c r="I277" t="b">
-        <v>1</v>
-      </c>
-      <c r="J277" t="s">
-        <v>921</v>
-      </c>
-      <c r="K277" t="s">
-        <v>809</v>
-      </c>
-      <c r="L277" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A278" t="s">
-        <v>898</v>
-      </c>
-      <c r="B278" t="s">
-        <v>899</v>
-      </c>
-      <c r="C278" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D278" t="s">
-        <v>900</v>
-      </c>
-      <c r="E278" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F278" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H278" t="s">
-        <v>901</v>
-      </c>
-      <c r="I278" t="b">
-        <v>1</v>
-      </c>
-      <c r="J278" t="s">
-        <v>922</v>
-      </c>
-      <c r="K278" t="s">
-        <v>809</v>
-      </c>
-      <c r="L278" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A279" t="s">
-        <v>902</v>
-      </c>
-      <c r="B279" t="s">
-        <v>903</v>
-      </c>
-      <c r="C279" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D279" t="s">
-        <v>904</v>
-      </c>
-      <c r="E279" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F279" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H279" t="s">
-        <v>887</v>
-      </c>
-      <c r="I279" t="b">
-        <v>1</v>
-      </c>
-      <c r="J279" t="s">
-        <v>923</v>
-      </c>
-      <c r="K279" t="s">
-        <v>809</v>
-      </c>
-      <c r="L279" t="s">
         <v>803</v>
       </c>
     </row>

</xml_diff>